<commit_message>
thêm chức năng thêm, sửa xóa,  thêm bằng excel cho quản lý từ vựng
</commit_message>
<xml_diff>
--- a/client/public/templates/vocabularies.xlsx
+++ b/client/public/templates/vocabularies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ki2Nam3\CongNghePhanMemHuongDoiTuong\project\StudyToeicWeb\client\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4661D2CB-57CF-4171-AE14-9B20227D35F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC9D419-3706-4614-8020-C0EE57B3386C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,30 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>content</t>
   </si>
@@ -298,7 +276,67 @@
     <t>cáo</t>
   </si>
   <si>
-    <t>client\public\templates\imageTest\avt.png</t>
+    <t>Ư</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/3a/Cat03.jpg/1200px-Cat03.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/37/African_Bush_Elephant.jpg/1200px-African_Bush_Elephant.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/7/73/Lion_waiting_in_Namibia.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/3f/Walking_tiger_female.jpg/1200px-Walking_tiger_female.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/43/Bonnet_macaque_%28Macaca_radiata%29_Photograph_By_Shantanu_Kuveskar.jpg/1200px-Bonnet_macaque_%28Macaca_radiata%29_Photograph_By_Shantanu_Kuveskar.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/e/e3/Plains_Zebra_Equus_quagga.jpg/1200px-Plains_Zebra_Equus_quagga.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/9/9e/Giraffe_Mikumi_National_Park.jpg/1200px-Giraffe_Mikumi_National_Park.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/00/Eunectes_notaeus_Pantanal_Brazil_2.jpg/1200px-Eunectes_notaeus_Pantanal_Brazil_2.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/45/Eopsaltria_australis_-_Mogo_Campground.jpg/640px-Eopsaltria_australis_-_Mogo_Campground.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/6/62/Clownfish_in_Andaman_Coral_Reef.jpg/1200px-Clownfish_in_Andaman_Coral_Reef.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/1/1f/Oryctolagus_cuniculus_Rcdo.jpg/1200px-Oryctolagus_cuniculus_Rcdo.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/1/10/Tursiops_truncatus_01.jpg/1200px-Tursiops_truncatus_01.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0c/Kangaroo_Australia_01_11_2008_-_retouch.jpg/800px-Kangaroo_Australia_01_11_2008_-_retouch.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0d/Aptenodytes_forsteri_-Snow_Hill_Island%2C_Antarctica_-adults_and_juvenile-8.jpg/1200px-Aptenodytes_forsteri_-Snow_Hill_Island%2C_Antarctica_-adults_and_juvenile-8.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0f/Grosser_Panda.JPG/1200px-Grosser_Panda.JPG</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/49/Koala_climbing_tree.jpg/800px-Koala_climbing_tree.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b3/Hipop%C3%B3tamo_%28Hippopotamus_amphibius%29%2C_parque_nacional_de_Chobe%2C_Botsuana%2C_2018-07-28%2C_DD_82.jpg/1200px-Hipop%C3%B3tamo_%28Hippopotamus_amphibius%29%2C_parque_nacional_de_Chobe%2C_Botsuana%2C_2018-07-28%2C_DD_82.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/5f/Kolm%C3%A5rden_Wolf.jpg/1200px-Kolm%C3%A5rden_Wolf.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Fox_-_British_Wildlife_Centre_%2817429406401%29.jpg/1200px-Fox_-_British_Wildlife_Centre_%2817429406401%29.jpg </t>
+  </si>
+  <si>
+    <t>https://byvn.net/Ty62</t>
   </si>
 </sst>
 </file>
@@ -362,70 +400,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,8 +711,8 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="F2" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -756,7 +730,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -773,7 +747,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -790,7 +764,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -807,7 +781,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -824,7 +798,7 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -841,7 +815,7 @@
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,7 +829,7 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -872,7 +846,7 @@
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -889,7 +863,7 @@
         <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -906,7 +880,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -923,7 +897,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,7 +914,7 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -957,7 +931,7 @@
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -971,10 +945,10 @@
         <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -988,10 +962,10 @@
         <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1005,10 +979,10 @@
         <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1022,10 +996,10 @@
         <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1039,10 +1013,10 @@
         <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1056,10 +1030,18 @@
         <v>63</v>
       </c>
       <c r="F21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{CE36689E-BC63-41E7-9D9A-34869EF2EB6A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chỉnh sửa database, xóa slug
</commit_message>
<xml_diff>
--- a/client/public/templates/vocabularies.xlsx
+++ b/client/public/templates/vocabularies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ki2Nam3\CongNghePhanMemHuongDoiTuong\project\StudyToeicWeb\client\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC9D419-3706-4614-8020-C0EE57B3386C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DDD50E-54E9-4EA4-A74C-738F5079AEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
   <si>
     <t>content</t>
   </si>
@@ -327,16 +327,10 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/49/Koala_climbing_tree.jpg/800px-Koala_climbing_tree.jpg</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b3/Hipop%C3%B3tamo_%28Hippopotamus_amphibius%29%2C_parque_nacional_de_Chobe%2C_Botsuana%2C_2018-07-28%2C_DD_82.jpg/1200px-Hipop%C3%B3tamo_%28Hippopotamus_amphibius%29%2C_parque_nacional_de_Chobe%2C_Botsuana%2C_2018-07-28%2C_DD_82.jpg</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/5f/Kolm%C3%A5rden_Wolf.jpg/1200px-Kolm%C3%A5rden_Wolf.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/1/16/Fox_-_British_Wildlife_Centre_%2817429406401%29.jpg/1200px-Fox_-_British_Wildlife_Centre_%2817429406401%29.jpg </t>
-  </si>
-  <si>
-    <t>https://byvn.net/Ty62</t>
   </si>
 </sst>
 </file>
@@ -668,7 +662,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -729,7 +723,7 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -995,8 +989,8 @@
       <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="F19" t="s">
-        <v>100</v>
+      <c r="F19" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1013,7 +1007,7 @@
         <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1030,7 +1024,7 @@
         <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -1041,6 +1035,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{CE36689E-BC63-41E7-9D9A-34869EF2EB6A}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{EE8954DA-128F-4487-A6D9-7A5B8E9B83B6}"/>
+    <hyperlink ref="F19" r:id="rId3" xr:uid="{0DD47B46-327F-4E31-9410-EC3A04EE2602}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>